<commit_message>
adding the readme file
</commit_message>
<xml_diff>
--- a/Simulations/sim_data/sim_output/k_tr_analysis.xlsx
+++ b/Simulations/sim_data/sim_output/k_tr_analysis.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -498,22 +498,22 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>5.7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>53717.3</v>
+        <v>28537.6</v>
       </c>
       <c r="D3" t="n">
-        <v>1104.46</v>
+        <v>1104.71</v>
       </c>
       <c r="E3" t="n">
-        <v>2.502854729106819</v>
+        <v>9.03304780150931</v>
       </c>
       <c r="F3" t="n">
-        <v>-2618.588650893631</v>
+        <v>3488.856245539169</v>
       </c>
       <c r="G3" t="n">
-        <v>0.08907416382829714</v>
+        <v>0.04393029047195163</v>
       </c>
     </row>
     <row r="4">
@@ -521,435 +521,159 @@
         <v>1</v>
       </c>
       <c r="B4" t="n">
-        <v>5.9</v>
+        <v>9</v>
       </c>
       <c r="C4" t="n">
-        <v>41513.5</v>
+        <v>4548.28</v>
       </c>
       <c r="D4" t="n">
-        <v>1104.58</v>
+        <v>1104.95</v>
       </c>
       <c r="E4" t="n">
-        <v>2.81510133284616</v>
+        <v>5.405405405405403</v>
       </c>
       <c r="F4" t="n">
-        <v>-11062.19081767158</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0.5833076822479319</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5" t="n">
-        <v>6.1</v>
+        <v>4.5</v>
       </c>
       <c r="C5" t="n">
-        <v>12853.7</v>
+        <v>77866.89999999999</v>
       </c>
       <c r="D5" t="n">
-        <v>1104.87</v>
+        <v>1104.22</v>
       </c>
       <c r="E5" t="n">
-        <v>5.260501144066696</v>
+        <v>14.89908603320762</v>
       </c>
       <c r="F5" t="n">
-        <v>3973.166814619847</v>
+        <v>814.8095496962055</v>
       </c>
       <c r="G5" t="n">
-        <v>0.2945045525441913</v>
+        <v>0.002159079296863986</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B6" t="n">
-        <v>6.3</v>
+        <v>6</v>
       </c>
       <c r="C6" t="n">
-        <v>7556.22</v>
+        <v>63436.3</v>
       </c>
       <c r="D6" t="n">
-        <v>1104.92</v>
+        <v>1104.37</v>
       </c>
       <c r="E6" t="n">
-        <v>7.155026945042359e-05</v>
+        <v>1.087776644263217</v>
       </c>
       <c r="F6" t="n">
-        <v>16168706.60404517</v>
+        <v>-4788.494929740694</v>
       </c>
       <c r="G6" t="n">
-        <v>0.06059094770121931</v>
+        <v>0.0906512619967581</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
+        <v>2</v>
+      </c>
+      <c r="B7" t="n">
+        <v>9</v>
+      </c>
+      <c r="C7" t="n">
+        <v>4548.28</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1104.95</v>
+      </c>
+      <c r="E7" t="n">
+        <v>5.405405405405403</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
         <v>1</v>
-      </c>
-      <c r="B7" t="n">
-        <v>6.5</v>
-      </c>
-      <c r="C7" t="n">
-        <v>7986.76</v>
-      </c>
-      <c r="D7" t="n">
-        <v>1104.92</v>
-      </c>
-      <c r="E7" t="n">
-        <v>50.03221384379605</v>
-      </c>
-      <c r="F7" t="n">
-        <v>932.0321117433276</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0.04563689974188601</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B8" t="n">
-        <v>9</v>
+        <v>4.5</v>
       </c>
       <c r="C8" t="n">
-        <v>4548.28</v>
+        <v>70813.8</v>
       </c>
       <c r="D8" t="n">
-        <v>1104.95</v>
+        <v>1104.29</v>
       </c>
       <c r="E8" t="n">
-        <v>5.405405405405403</v>
+        <v>1.46405849275004</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>-3804.435037701195</v>
       </c>
       <c r="G8" t="n">
-        <v>1</v>
+        <v>0.09212360213787463</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B9" t="n">
-        <v>4.5</v>
+        <v>6</v>
       </c>
       <c r="C9" t="n">
-        <v>77866.89999999999</v>
+        <v>36763.4</v>
       </c>
       <c r="D9" t="n">
-        <v>1104.22</v>
+        <v>1104.63</v>
       </c>
       <c r="E9" t="n">
-        <v>14.89908603320762</v>
+        <v>6.115890524622755</v>
       </c>
       <c r="F9" t="n">
-        <v>814.8095496962055</v>
+        <v>2382.520309981491</v>
       </c>
       <c r="G9" t="n">
-        <v>0.002159079296863986</v>
+        <v>0.03704759944721769</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B10" t="n">
-        <v>5.7</v>
+        <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>71521.10000000001</v>
+        <v>4548.28</v>
       </c>
       <c r="D10" t="n">
-        <v>1104.28</v>
+        <v>1104.95</v>
       </c>
       <c r="E10" t="n">
-        <v>0.0008804811497622391</v>
+        <v>5.405405405405403</v>
       </c>
       <c r="F10" t="n">
-        <v>-779478.8092512469</v>
+        <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>0.007106462151890813</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>2</v>
-      </c>
-      <c r="B11" t="n">
-        <v>5.9</v>
-      </c>
-      <c r="C11" t="n">
-        <v>71629.8</v>
-      </c>
-      <c r="D11" t="n">
-        <v>1104.28</v>
-      </c>
-      <c r="E11" t="n">
-        <v>18.52508539354778</v>
-      </c>
-      <c r="F11" t="n">
-        <v>9214.100460778536</v>
-      </c>
-      <c r="G11" t="n">
-        <v>0.2757949618927992</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>2</v>
-      </c>
-      <c r="B12" t="n">
-        <v>6.1</v>
-      </c>
-      <c r="C12" t="n">
-        <v>60464.3</v>
-      </c>
-      <c r="D12" t="n">
-        <v>1104.4</v>
-      </c>
-      <c r="E12" t="n">
-        <v>3.178985523477124</v>
-      </c>
-      <c r="F12" t="n">
-        <v>11695.34159363227</v>
-      </c>
-      <c r="G12" t="n">
-        <v>0.6260593475771274</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>2</v>
-      </c>
-      <c r="B13" t="n">
-        <v>6.3</v>
-      </c>
-      <c r="C13" t="n">
-        <v>20565.6</v>
-      </c>
-      <c r="D13" t="n">
-        <v>1104.79</v>
-      </c>
-      <c r="E13" t="n">
-        <v>5.741321387535455</v>
-      </c>
-      <c r="F13" t="n">
-        <v>-7583.066039531271</v>
-      </c>
-      <c r="G13" t="n">
-        <v>0.4531770870522079</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>2</v>
-      </c>
-      <c r="B14" t="n">
-        <v>6.5</v>
-      </c>
-      <c r="C14" t="n">
-        <v>8236.34</v>
-      </c>
-      <c r="D14" t="n">
-        <v>1104.92</v>
-      </c>
-      <c r="E14" t="n">
-        <v>5.53406960535952e-05</v>
-      </c>
-      <c r="F14" t="n">
-        <v>39396421.20489686</v>
-      </c>
-      <c r="G14" t="n">
-        <v>0.2388310882350358</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>2</v>
-      </c>
-      <c r="B15" t="n">
-        <v>9</v>
-      </c>
-      <c r="C15" t="n">
-        <v>4548.28</v>
-      </c>
-      <c r="D15" t="n">
-        <v>1104.95</v>
-      </c>
-      <c r="E15" t="n">
-        <v>5.405405405405403</v>
-      </c>
-      <c r="F15" t="n">
-        <v>0</v>
-      </c>
-      <c r="G15" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>3</v>
-      </c>
-      <c r="B16" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="C16" t="n">
-        <v>70813.8</v>
-      </c>
-      <c r="D16" t="n">
-        <v>1104.29</v>
-      </c>
-      <c r="E16" t="n">
-        <v>1.46405849275004</v>
-      </c>
-      <c r="F16" t="n">
-        <v>-3804.435037701195</v>
-      </c>
-      <c r="G16" t="n">
-        <v>0.09212360213787463</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>3</v>
-      </c>
-      <c r="B17" t="n">
-        <v>5.7</v>
-      </c>
-      <c r="C17" t="n">
-        <v>65811.5</v>
-      </c>
-      <c r="D17" t="n">
-        <v>1104.34</v>
-      </c>
-      <c r="E17" t="n">
-        <v>4.194162224903733</v>
-      </c>
-      <c r="F17" t="n">
-        <v>-588.2965640972723</v>
-      </c>
-      <c r="G17" t="n">
-        <v>0.005054425795419371</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>3</v>
-      </c>
-      <c r="B18" t="n">
-        <v>5.9</v>
-      </c>
-      <c r="C18" t="n">
-        <v>47733</v>
-      </c>
-      <c r="D18" t="n">
-        <v>1104.52</v>
-      </c>
-      <c r="E18" t="n">
-        <v>126.180858854266</v>
-      </c>
-      <c r="F18" t="n">
-        <v>-5967.466757611687</v>
-      </c>
-      <c r="G18" t="n">
-        <v>0.01109130623015475</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>3</v>
-      </c>
-      <c r="B19" t="n">
-        <v>6.1</v>
-      </c>
-      <c r="C19" t="n">
-        <v>19603.6</v>
-      </c>
-      <c r="D19" t="n">
-        <v>1104.8</v>
-      </c>
-      <c r="E19" t="n">
-        <v>2.640860191309929</v>
-      </c>
-      <c r="F19" t="n">
-        <v>-8361.566939392211</v>
-      </c>
-      <c r="G19" t="n">
-        <v>0.2892547955939947</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>3</v>
-      </c>
-      <c r="B20" t="n">
-        <v>6.3</v>
-      </c>
-      <c r="C20" t="n">
-        <v>7040.22</v>
-      </c>
-      <c r="D20" t="n">
-        <v>1104.93</v>
-      </c>
-      <c r="E20" t="n">
-        <v>4.197888879914294e-05</v>
-      </c>
-      <c r="F20" t="n">
-        <v>85344619.06330547</v>
-      </c>
-      <c r="G20" t="n">
-        <v>0.382609827546984</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>3</v>
-      </c>
-      <c r="B21" t="n">
-        <v>6.5</v>
-      </c>
-      <c r="C21" t="n">
-        <v>5171.18</v>
-      </c>
-      <c r="D21" t="n">
-        <v>1104.95</v>
-      </c>
-      <c r="E21" t="n">
-        <v>7.38168631390351</v>
-      </c>
-      <c r="F21" t="n">
-        <v>1125.811406416023</v>
-      </c>
-      <c r="G21" t="n">
-        <v>0.1740056362660986</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="n">
-        <v>3</v>
-      </c>
-      <c r="B22" t="n">
-        <v>9</v>
-      </c>
-      <c r="C22" t="n">
-        <v>4548.28</v>
-      </c>
-      <c r="D22" t="n">
-        <v>1104.95</v>
-      </c>
-      <c r="E22" t="n">
-        <v>5.405405405405403</v>
-      </c>
-      <c r="F22" t="n">
-        <v>0</v>
-      </c>
-      <c r="G22" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>